<commit_message>
Updating Survey Data Analysis Spreadsheet
</commit_message>
<xml_diff>
--- a/data/Survey Data Analysis.xlsx
+++ b/data/Survey Data Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kamden Chew\Desktop\School Work\Senior Year\Quarter 2\CSE 403\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{160C12AF-5F5C-4228-BE4E-D936AC878EF2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F960FBF7-1ED0-47EA-A840-4A0690C7F607}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{77A3A7D4-3AA6-4712-8ED6-7E459DD1EF7A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="114">
   <si>
     <t>Responses:</t>
   </si>
@@ -45,308 +45,341 @@
     <t>GitUp</t>
   </si>
   <si>
-    <t>Question 1</t>
-  </si>
-  <si>
-    <t>Question 2</t>
-  </si>
-  <si>
-    <t>Question 3</t>
-  </si>
-  <si>
-    <t>Question 4</t>
-  </si>
-  <si>
-    <t>Question 5</t>
-  </si>
-  <si>
-    <t>Question 6</t>
-  </si>
-  <si>
-    <t>Question 7</t>
-  </si>
-  <si>
-    <t>Question 8</t>
-  </si>
-  <si>
-    <t>Question 9</t>
-  </si>
-  <si>
-    <t>Question 10</t>
-  </si>
-  <si>
-    <t>Question 11</t>
-  </si>
-  <si>
-    <t>Question 12</t>
-  </si>
-  <si>
-    <t>Question 13</t>
-  </si>
-  <si>
-    <t>Question 14</t>
-  </si>
-  <si>
-    <t>Question 15</t>
-  </si>
-  <si>
-    <t>Question 16</t>
-  </si>
-  <si>
-    <t>Question 17</t>
-  </si>
-  <si>
-    <t>Question 18</t>
-  </si>
-  <si>
-    <t>Question 19</t>
-  </si>
-  <si>
-    <t>Question 20</t>
-  </si>
-  <si>
-    <t>Question 21</t>
-  </si>
-  <si>
-    <t>Question 22</t>
-  </si>
-  <si>
-    <t>Question 23</t>
-  </si>
-  <si>
-    <t>Question 24</t>
-  </si>
-  <si>
-    <t>Question 25</t>
-  </si>
-  <si>
-    <t>Question 26</t>
-  </si>
-  <si>
-    <t>Question 27</t>
-  </si>
-  <si>
-    <t>Question 28</t>
-  </si>
-  <si>
-    <t>Question 29</t>
-  </si>
-  <si>
-    <t>Question 30</t>
-  </si>
-  <si>
-    <t>Question 31</t>
-  </si>
-  <si>
-    <t>Question 32</t>
-  </si>
-  <si>
-    <t>Question 33</t>
-  </si>
-  <si>
-    <t>Question 34</t>
-  </si>
-  <si>
-    <t>Question 35</t>
-  </si>
-  <si>
-    <t>Question 36</t>
-  </si>
-  <si>
-    <t>Question 37</t>
-  </si>
-  <si>
-    <t>Question 38</t>
-  </si>
-  <si>
-    <t>Question 39</t>
-  </si>
-  <si>
-    <t>Question 40</t>
-  </si>
-  <si>
-    <t>Question 41</t>
-  </si>
-  <si>
-    <t>Question 42</t>
-  </si>
-  <si>
-    <t>Question 43</t>
-  </si>
-  <si>
-    <t>Question 44</t>
-  </si>
-  <si>
-    <t>Question 45</t>
-  </si>
-  <si>
-    <t>Question 46</t>
-  </si>
-  <si>
-    <t>Question 47</t>
-  </si>
-  <si>
-    <t>Question 48</t>
-  </si>
-  <si>
-    <t>Question 49</t>
-  </si>
-  <si>
-    <t>Question 50</t>
-  </si>
-  <si>
-    <t>Question 51</t>
-  </si>
-  <si>
-    <t>Question 52</t>
-  </si>
-  <si>
-    <t>Question 53</t>
-  </si>
-  <si>
-    <t>Question 54</t>
-  </si>
-  <si>
-    <t>Question 55</t>
-  </si>
-  <si>
-    <t>Question 56</t>
-  </si>
-  <si>
-    <t>Question 57</t>
-  </si>
-  <si>
-    <t>Question 58</t>
-  </si>
-  <si>
-    <t>Question 59</t>
-  </si>
-  <si>
-    <t>Question 60</t>
-  </si>
-  <si>
-    <t>Question 61</t>
-  </si>
-  <si>
-    <t>Question 62</t>
-  </si>
-  <si>
-    <t>Question 63</t>
-  </si>
-  <si>
-    <t>Question 64</t>
-  </si>
-  <si>
-    <t>Question 65</t>
-  </si>
-  <si>
-    <t>Question 66</t>
-  </si>
-  <si>
-    <t>Question 67</t>
-  </si>
-  <si>
-    <t>Question 68</t>
-  </si>
-  <si>
-    <t>Question 69</t>
-  </si>
-  <si>
-    <t>Question 70</t>
-  </si>
-  <si>
-    <t>Question 71</t>
-  </si>
-  <si>
-    <t>Question 72</t>
-  </si>
-  <si>
-    <t>Question 73</t>
-  </si>
-  <si>
-    <t>Question 74</t>
-  </si>
-  <si>
-    <t>Question 75</t>
-  </si>
-  <si>
-    <t>Question 76</t>
-  </si>
-  <si>
-    <t>Question 77</t>
-  </si>
-  <si>
-    <t>Question 78</t>
-  </si>
-  <si>
-    <t>Question 79</t>
-  </si>
-  <si>
-    <t>Question 80</t>
-  </si>
-  <si>
-    <t>Question 81</t>
-  </si>
-  <si>
-    <t>Question 82</t>
-  </si>
-  <si>
-    <t>Question 83</t>
-  </si>
-  <si>
-    <t>Question 84</t>
-  </si>
-  <si>
-    <t>Question 85</t>
-  </si>
-  <si>
-    <t>Question 86</t>
-  </si>
-  <si>
-    <t>Question 87</t>
-  </si>
-  <si>
-    <t>Question 88</t>
-  </si>
-  <si>
-    <t>Question 89</t>
-  </si>
-  <si>
-    <t>Question 90</t>
-  </si>
-  <si>
-    <t>Question 91</t>
-  </si>
-  <si>
-    <t>Question 92</t>
-  </si>
-  <si>
-    <t>Question 93</t>
-  </si>
-  <si>
-    <t>Question 94</t>
-  </si>
-  <si>
-    <t>Question 95</t>
-  </si>
-  <si>
-    <t>Question 96</t>
-  </si>
-  <si>
-    <t>Question 97</t>
-  </si>
-  <si>
-    <t>Question 98</t>
-  </si>
-  <si>
-    <t>Question 99</t>
+    <t>Git Tasks Completed</t>
+  </si>
+  <si>
+    <t>GitKraken Tasks Compelted</t>
+  </si>
+  <si>
+    <t>GitUp Tasks Completed</t>
+  </si>
+  <si>
+    <t>Responder 1</t>
+  </si>
+  <si>
+    <t>Responder 2</t>
+  </si>
+  <si>
+    <t>Responder 3</t>
+  </si>
+  <si>
+    <t>Responder 4</t>
+  </si>
+  <si>
+    <t>Responder 5</t>
+  </si>
+  <si>
+    <t>Responder 6</t>
+  </si>
+  <si>
+    <t>Responder 7</t>
+  </si>
+  <si>
+    <t>Responder 8</t>
+  </si>
+  <si>
+    <t>Responder 9</t>
+  </si>
+  <si>
+    <t>Responder 10</t>
+  </si>
+  <si>
+    <t>Responder 11</t>
+  </si>
+  <si>
+    <t>Responder 12</t>
+  </si>
+  <si>
+    <t>Responder 13</t>
+  </si>
+  <si>
+    <t>Responder 14</t>
+  </si>
+  <si>
+    <t>Responder 15</t>
+  </si>
+  <si>
+    <t>Responder 16</t>
+  </si>
+  <si>
+    <t>Responder 17</t>
+  </si>
+  <si>
+    <t>Responder 18</t>
+  </si>
+  <si>
+    <t>Responder 19</t>
+  </si>
+  <si>
+    <t>Responder 20</t>
+  </si>
+  <si>
+    <t>Responder 21</t>
+  </si>
+  <si>
+    <t>Responder 22</t>
+  </si>
+  <si>
+    <t>Responder 23</t>
+  </si>
+  <si>
+    <t>Responder 24</t>
+  </si>
+  <si>
+    <t>Responder 25</t>
+  </si>
+  <si>
+    <t>Responder 26</t>
+  </si>
+  <si>
+    <t>Responder 27</t>
+  </si>
+  <si>
+    <t>Responder 28</t>
+  </si>
+  <si>
+    <t>Responder 29</t>
+  </si>
+  <si>
+    <t>Responder 30</t>
+  </si>
+  <si>
+    <t>Responder 31</t>
+  </si>
+  <si>
+    <t>Responder 32</t>
+  </si>
+  <si>
+    <t>Responder 33</t>
+  </si>
+  <si>
+    <t>Responder 34</t>
+  </si>
+  <si>
+    <t>Responder 35</t>
+  </si>
+  <si>
+    <t>Responder 36</t>
+  </si>
+  <si>
+    <t>Responder 37</t>
+  </si>
+  <si>
+    <t>Responder 38</t>
+  </si>
+  <si>
+    <t>Responder 39</t>
+  </si>
+  <si>
+    <t>Responder 40</t>
+  </si>
+  <si>
+    <t>Responder 41</t>
+  </si>
+  <si>
+    <t>Responder 42</t>
+  </si>
+  <si>
+    <t>Responder 43</t>
+  </si>
+  <si>
+    <t>Responder 44</t>
+  </si>
+  <si>
+    <t>Responder 45</t>
+  </si>
+  <si>
+    <t>Responder 46</t>
+  </si>
+  <si>
+    <t>Responder 47</t>
+  </si>
+  <si>
+    <t>Responder 48</t>
+  </si>
+  <si>
+    <t>Responder 49</t>
+  </si>
+  <si>
+    <t>Responder 50</t>
+  </si>
+  <si>
+    <t>Responder 51</t>
+  </si>
+  <si>
+    <t>Responder 52</t>
+  </si>
+  <si>
+    <t>Responder 53</t>
+  </si>
+  <si>
+    <t>Responder 54</t>
+  </si>
+  <si>
+    <t>Responder 55</t>
+  </si>
+  <si>
+    <t>Responder 56</t>
+  </si>
+  <si>
+    <t>Responder 57</t>
+  </si>
+  <si>
+    <t>Responder 58</t>
+  </si>
+  <si>
+    <t>Responder 59</t>
+  </si>
+  <si>
+    <t>Responder 60</t>
+  </si>
+  <si>
+    <t>Responder 61</t>
+  </si>
+  <si>
+    <t>Responder 62</t>
+  </si>
+  <si>
+    <t>Responder 63</t>
+  </si>
+  <si>
+    <t>Responder 64</t>
+  </si>
+  <si>
+    <t>Responder 65</t>
+  </si>
+  <si>
+    <t>Responder 66</t>
+  </si>
+  <si>
+    <t>Responder 67</t>
+  </si>
+  <si>
+    <t>Responder 68</t>
+  </si>
+  <si>
+    <t>Responder 69</t>
+  </si>
+  <si>
+    <t>Responder 70</t>
+  </si>
+  <si>
+    <t>Responder 71</t>
+  </si>
+  <si>
+    <t>Responder 72</t>
+  </si>
+  <si>
+    <t>Responder 73</t>
+  </si>
+  <si>
+    <t>Responder 74</t>
+  </si>
+  <si>
+    <t>Responder 75</t>
+  </si>
+  <si>
+    <t>Responder 76</t>
+  </si>
+  <si>
+    <t>Responder 77</t>
+  </si>
+  <si>
+    <t>Responder 78</t>
+  </si>
+  <si>
+    <t>Responder 79</t>
+  </si>
+  <si>
+    <t>Responder 80</t>
+  </si>
+  <si>
+    <t>Responder 81</t>
+  </si>
+  <si>
+    <t>Responder 82</t>
+  </si>
+  <si>
+    <t>Responder 83</t>
+  </si>
+  <si>
+    <t>Responder 84</t>
+  </si>
+  <si>
+    <t>Responder 85</t>
+  </si>
+  <si>
+    <t>Responder 86</t>
+  </si>
+  <si>
+    <t>Responder 87</t>
+  </si>
+  <si>
+    <t>Responder 88</t>
+  </si>
+  <si>
+    <t>Responder 89</t>
+  </si>
+  <si>
+    <t>Responder 90</t>
+  </si>
+  <si>
+    <t>Responder 91</t>
+  </si>
+  <si>
+    <t>Responder 92</t>
+  </si>
+  <si>
+    <t>Responder 93</t>
+  </si>
+  <si>
+    <t>Responder 94</t>
+  </si>
+  <si>
+    <t>Responder 95</t>
+  </si>
+  <si>
+    <t>Responder 96</t>
+  </si>
+  <si>
+    <t>Responder 97</t>
+  </si>
+  <si>
+    <t>Responder 98</t>
+  </si>
+  <si>
+    <t>Responder 99</t>
+  </si>
+  <si>
+    <t>Responder 100</t>
+  </si>
+  <si>
+    <t>Most Functional Vote</t>
+  </si>
+  <si>
+    <t>Easiest to Use Vote</t>
+  </si>
+  <si>
+    <t>Best Overall Vote</t>
+  </si>
+  <si>
+    <t>Average # of Tasks Completed in 30 Minutes:</t>
+  </si>
+  <si>
+    <t>Most Functional # of votes:</t>
+  </si>
+  <si>
+    <t>Easiest to Use # of votes:</t>
+  </si>
+  <si>
+    <t>Best Overall # of votes:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -354,13 +387,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -375,8 +420,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,8 +476,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Survey Results</a:t>
+              <a:t>VCS Tool vs. Average Tasks Completed</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> in 30 Minutes</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -485,7 +537,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$1:$H$1</c:f>
+              <c:f>Sheet1!$H$2:$J$2</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -502,7 +554,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$H$2</c:f>
+              <c:f>Sheet1!$H$3:$J$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -806,7 +858,1368 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Most</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Functional Votes</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$H$6:$J$6</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Git</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GitKraken</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>GitUp</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$7:$J$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-38AE-40FC-A075-D719EB655250}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="520339304"/>
+        <c:axId val="520339632"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="520339304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>VCS Tool</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="520339632"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="520339632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Votes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="520339304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Easiest to Use Votes</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$H$10:$J$10</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Git</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GitKraken</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>GitUp</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$11:$J$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3AEC-4805-A0C3-EB17AD375891}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="520336352"/>
+        <c:axId val="520337336"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="520336352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>VCS Tool</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="520337336"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="520337336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Votes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="520336352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Best Overall Votes</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$H$14:$J$14</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Git</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GitKraken</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>GitUp</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$15:$J$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-956C-45D8-A987-505138B6F797}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="400859848"/>
+        <c:axId val="400862144"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="400859848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>VCS Tool</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="400862144"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="400862144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Votes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="400859848"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1349,20 +2762,1529 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>144780</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>149542</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>115252</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>449580</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>174307</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>590549</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>132397</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1382,6 +4304,114 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>130492</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>107632</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>427672</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>132397</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7AD1540-7133-469C-BD20-8C9F048DBFB8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1039177</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>67627</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>574357</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>92392</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76CA4235-8230-43CE-8791-1EDD3F916F24}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>136207</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>103822</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>446722</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>130492</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DBFD733-8305-4C4E-85A4-1F691C185F0A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1687,554 +4717,656 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6166FB27-E96C-40AA-B58A-7FBDE994DEC3}">
-  <dimension ref="A1:H100"/>
+  <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.44140625" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" customWidth="1"/>
-    <col min="7" max="7" width="23.5546875" customWidth="1"/>
-    <col min="8" max="8" width="20" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="19.77734375" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="9" max="9" width="22.5546875" customWidth="1"/>
+    <col min="10" max="10" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="I2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="J2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="e">
+        <f xml:space="preserve"> AVERAGE(B2:B101)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I3" t="e">
+        <f xml:space="preserve"> AVERAGE(C2:C101)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J3" t="e">
+        <f xml:space="preserve"> AVERAGE(D2:D101)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" t="s">
         <v>1</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I6" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2">
-        <f xml:space="preserve"> SUM(B2:B100)</f>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="1">
+        <f>COUNTIF(E2:E101,"Git")</f>
         <v>0</v>
       </c>
-      <c r="G2">
-        <f xml:space="preserve"> SUM(C2:C100)</f>
+      <c r="I7">
+        <f>COUNTIF(E2:E101,"GitKraken")</f>
         <v>0</v>
       </c>
-      <c r="H2">
-        <f xml:space="preserve"> SUM(D2:D100)</f>
+      <c r="J7">
+        <f>COUNTIF(E2:E101,"GitUp")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="H10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" t="s">
+        <v>2</v>
+      </c>
+      <c r="J10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="H11" s="1">
+        <f>COUNTIF(F2:F101,"Git")</f>
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <f>COUNTIF(F2:F101,"GitKraken")</f>
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <f>COUNTIF(F2:F101,"GitUp")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="H14" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" t="s">
+        <v>2</v>
+      </c>
+      <c r="J14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="H15" s="1">
+        <f>COUNTIF(G2:G101,"Git")</f>
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <f>COUNTIF(G2:G101,"GitKraken")</f>
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <f>COUNTIF(G2:G101,"GitUp")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>102</v>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reupload of Survey Data Analysis with sample data
</commit_message>
<xml_diff>
--- a/data/Survey Data Analysis.xlsx
+++ b/data/Survey Data Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kamden Chew\Desktop\School Work\Senior Year\Quarter 2\CSE 403\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F960FBF7-1ED0-47EA-A840-4A0690C7F607}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6092056F-8CFA-489C-B81E-929A176D7FAA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{77A3A7D4-3AA6-4712-8ED6-7E459DD1EF7A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="114">
   <si>
     <t>Responses:</t>
   </si>
@@ -559,13 +559,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -976,10 +976,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1391,10 +1391,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1803,10 +1803,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4720,7 +4720,7 @@
   <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4769,6 +4769,24 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
       <c r="H2" t="s">
         <v>1</v>
       </c>
@@ -4783,23 +4801,59 @@
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="H3" t="e">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3">
         <f xml:space="preserve"> AVERAGE(B2:B101)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I3" t="e">
+        <v>2</v>
+      </c>
+      <c r="I3">
         <f xml:space="preserve"> AVERAGE(C2:C101)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J3" t="e">
+        <v>3</v>
+      </c>
+      <c r="J3">
         <f xml:space="preserve"> AVERAGE(D2:D101)</f>
-        <v>#DIV/0!</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -4831,11 +4885,11 @@
       </c>
       <c r="H7" s="1">
         <f>COUNTIF(E2:E101,"Git")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I7">
         <f>COUNTIF(E2:E101,"GitKraken")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7">
         <f>COUNTIF(E2:E101,"GitUp")</f>
@@ -4881,11 +4935,11 @@
       </c>
       <c r="I11">
         <f>COUNTIF(F2:F101,"GitKraken")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11">
         <f>COUNTIF(F2:F101,"GitUp")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -4927,11 +4981,11 @@
       </c>
       <c r="I15">
         <f>COUNTIF(G2:G101,"GitKraken")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15">
         <f>COUNTIF(G2:G101,"GitUp")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>